<commit_message>
Project Plan v1 complete
</commit_message>
<xml_diff>
--- a/HW 1/Project Plan Template.xlsx
+++ b/HW 1/Project Plan Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25260" windowHeight="12200" activeTab="1"/>
+    <workbookView xWindow="180" yWindow="0" windowWidth="25260" windowHeight="12200" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Project Timeline" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="147">
   <si>
     <t>Project Start</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>Further develop this project plan (it is part of HW1) - THINK through your time management and what you will accomplish as the weeks progress.</t>
-  </si>
-  <si>
-    <t>fill me in…</t>
   </si>
   <si>
     <t>E-R diagrams complete with supporting documentation if explanation is required for anything you document in your diagrams.</t>
@@ -138,9 +135,6 @@
 Final UML Diagrams</t>
   </si>
   <si>
-    <t xml:space="preserve">Draft database design </t>
-  </si>
-  <si>
     <t>Complete initial (ie. first pass feedback) peer reviews</t>
   </si>
   <si>
@@ -168,9 +162,6 @@
   </si>
   <si>
     <t>Complete final peer evaluation forms and submit</t>
-  </si>
-  <si>
-    <t>Git er dun!</t>
   </si>
   <si>
     <t>Week</t>
@@ -378,34 +369,16 @@
     <t>Complete wireframe mock-ups!</t>
   </si>
   <si>
-    <t>9/26-9/27</t>
-  </si>
-  <si>
-    <t>Documentation for Mock-ups</t>
-  </si>
-  <si>
     <t>Finalization (Project plan)</t>
   </si>
   <si>
     <t>Make final edits to project plan (other)</t>
   </si>
   <si>
-    <t>Delagate weekly tasks</t>
-  </si>
-  <si>
-    <t>Give specific tasks before meeting Friday</t>
-  </si>
-  <si>
     <t>Finalize Database Draft</t>
   </si>
   <si>
-    <t>Meeting to Finalize Database draft</t>
-  </si>
-  <si>
     <t>Begin Database Design</t>
-  </si>
-  <si>
-    <t>10/6-10/8</t>
   </si>
   <si>
     <t>ERD Complete</t>
@@ -453,6 +426,73 @@
   </si>
   <si>
     <t>Dev team</t>
+  </si>
+  <si>
+    <t>Documentation for Mock-ups completed</t>
+  </si>
+  <si>
+    <t>Finalization (UML)</t>
+  </si>
+  <si>
+    <t>Finish the UML</t>
+  </si>
+  <si>
+    <t>Create initial database mockup</t>
+  </si>
+  <si>
+    <t>Finalize Database draft</t>
+  </si>
+  <si>
+    <t>Build initial UI</t>
+  </si>
+  <si>
+    <t>Implement initial UI from mockups</t>
+  </si>
+  <si>
+    <t>Document UI</t>
+  </si>
+  <si>
+    <t>Documentation of initial UI</t>
+  </si>
+  <si>
+    <t>Have Network design specfications complete</t>
+  </si>
+  <si>
+    <t>Have all specifications identified</t>
+  </si>
+  <si>
+    <t>Documentation of network design</t>
+  </si>
+  <si>
+    <t>Document network design</t>
+  </si>
+  <si>
+    <t>Dev Team + Matt Marak.</t>
+  </si>
+  <si>
+    <t>Network design finalized</t>
+  </si>
+  <si>
+    <t>Finalize IT requirements and Network design drafts</t>
+  </si>
+  <si>
+    <t>Matt Marak.</t>
+  </si>
+  <si>
+    <t>IT Hardware installed</t>
+  </si>
+  <si>
+    <t>Hardware setup + server setup 
+External dependencies installed and configured</t>
+  </si>
+  <si>
+    <t>Database built and tested</t>
+  </si>
+  <si>
+    <t>Database initialized and confirmed operational</t>
+  </si>
+  <si>
+    <t>Put em in a coffin entire thing is AWPerational</t>
   </si>
 </sst>
 </file>
@@ -542,13 +582,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -599,8 +632,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -630,8 +669,20 @@
         <bgColor theme="3" tint="9.9948118533890809E-2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBFCF4"/>
+        <bgColor rgb="FF3C3F53"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -701,74 +752,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="2" tint="-9.9948118533890809E-2"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2" tint="-9.9948118533890809E-2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="3"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="2" tint="-9.9948118533890809E-2"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2" tint="-9.9948118533890809E-2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="3"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="2" tint="-9.9948118533890809E-2"/>
-      </top>
-      <bottom style="thick">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="2" tint="-9.9948118533890809E-2"/>
-      </top>
-      <bottom style="thick">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="3"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="2" tint="-9.9948118533890809E-2"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="2" tint="-9.9948118533890809E-2"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -820,8 +803,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -831,44 +885,50 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -918,24 +978,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="6" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -945,58 +990,40 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="6" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="5" applyAlignment="1">
@@ -1005,20 +1032,74 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="5" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="5" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" xfId="5" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" xfId="5" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="5" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="21">
     <cellStyle name="Calculation" xfId="6" builtinId="22"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
@@ -1026,6 +1107,7 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
@@ -1035,6 +1117,7 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Output" xfId="5" builtinId="21"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -1674,8 +1757,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2109293016"/>
-        <c:axId val="2109290072"/>
+        <c:axId val="2120554024"/>
+        <c:axId val="2120551080"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1846,11 +1929,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2109283080"/>
-        <c:axId val="2109286936"/>
+        <c:axId val="2120544376"/>
+        <c:axId val="2120548008"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2109283080"/>
+        <c:axId val="2120544376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1890,7 +1973,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109286936"/>
+        <c:crossAx val="2120548008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1901,7 +1984,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2109286936"/>
+        <c:axId val="2120548008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1911,12 +1994,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109283080"/>
+        <c:crossAx val="2120544376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2109290072"/>
+        <c:axId val="2120551080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1926,12 +2009,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109293016"/>
+        <c:crossAx val="2120554024"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2109293016"/>
+        <c:axId val="2120554024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1941,7 +2024,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109290072"/>
+        <c:crossAx val="2120551080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2882,543 +2965,605 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A31" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="23" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="23" customWidth="1"/>
-    <col min="3" max="3" width="58.6640625" style="23" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" style="17" customWidth="1"/>
-    <col min="5" max="5" width="92" style="23" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="23"/>
+    <col min="1" max="1" width="15.5" style="60" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="61" customWidth="1"/>
+    <col min="3" max="3" width="58.6640625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="48" customWidth="1"/>
+    <col min="5" max="5" width="92" style="18" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="18" customFormat="1">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:5" s="17" customFormat="1">
+      <c r="A1" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="46" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A2" s="19">
+    <row r="2" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A2" s="54">
         <v>42247</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="45" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="24" customFormat="1" ht="48">
-      <c r="A3" s="19">
+    <row r="3" spans="1:5" s="19" customFormat="1" ht="48">
+      <c r="A3" s="54">
         <v>42247</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="45" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A4" s="19">
+    <row r="4" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A4" s="54">
         <v>42247</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="45" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="24" customFormat="1" ht="24">
-      <c r="A5" s="19">
+    <row r="5" spans="1:5" s="19" customFormat="1" ht="24">
+      <c r="A5" s="54">
         <v>42251</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A6" s="54">
+        <v>42254</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="19" customFormat="1" ht="56" customHeight="1">
+      <c r="A7" s="54">
+        <v>42260</v>
+      </c>
+      <c r="B7" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" s="45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="19" customFormat="1" ht="72">
+      <c r="A8" s="54">
+        <v>42261</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A9" s="54">
+        <v>42265</v>
+      </c>
+      <c r="B9" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A10" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A11" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" s="55" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A12" s="54">
+        <v>42268</v>
+      </c>
+      <c r="B12" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="45"/>
+    </row>
+    <row r="13" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A13" s="54">
+        <v>42272</v>
+      </c>
+      <c r="B13" s="55" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="D5" s="26" t="s">
+    </row>
+    <row r="14" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A14" s="54">
+        <v>42274</v>
+      </c>
+      <c r="B14" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" s="45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A15" s="54">
+        <v>42275</v>
+      </c>
+      <c r="B15" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="45" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A6" s="19">
-        <v>42254</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="C6" s="24" t="s">
+    <row r="16" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A16" s="54">
+        <v>42279</v>
+      </c>
+      <c r="B16" s="55" t="s">
         <v>126</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="C16" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="D16" s="45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A17" s="54">
+        <v>42279</v>
+      </c>
+      <c r="B17" s="55" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="45" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="24" customFormat="1" ht="56" customHeight="1">
-      <c r="A7" s="19">
-        <v>42260</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="C7" s="24" t="s">
+    <row r="18" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A18" s="54">
+        <v>42282</v>
+      </c>
+      <c r="B18" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A19" s="54">
+        <v>42283</v>
+      </c>
+      <c r="B19" s="55" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D19" s="45" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="24" customFormat="1" ht="72">
-      <c r="A8" s="19">
-        <v>42261</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" s="26" t="s">
+    <row r="20" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A20" s="54">
+        <v>42286</v>
+      </c>
+      <c r="B20" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20" s="45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A21" s="54">
+        <v>42289</v>
+      </c>
+      <c r="B21" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" s="45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A22" s="54">
+        <v>42293</v>
+      </c>
+      <c r="B22" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22" s="45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A23" s="56">
+        <v>42293</v>
+      </c>
+      <c r="B23" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="49" t="s">
+        <v>135</v>
+      </c>
+      <c r="D23" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="E23" s="51"/>
+    </row>
+    <row r="24" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A24" s="54">
+        <v>42296</v>
+      </c>
+      <c r="B24" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="45" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A9" s="19">
-        <v>42265</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="D9" s="26" t="s">
+    <row r="25" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A25" s="54">
+        <v>42300</v>
+      </c>
+      <c r="B25" s="55" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="D25" s="45" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A26" s="54">
+        <v>42302</v>
+      </c>
+      <c r="B26" s="55" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="D26" s="45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A27" s="54">
+        <v>42305</v>
+      </c>
+      <c r="B27" s="55" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" s="62" t="s">
+        <v>143</v>
+      </c>
+      <c r="D27" s="45" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A28" s="54">
+        <v>42307</v>
+      </c>
+      <c r="B28" s="55" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="D28" s="45" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A10" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A11" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="D11" s="26" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A12" s="19">
-        <v>42268</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="26"/>
-    </row>
-    <row r="13" spans="1:5" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A13" s="19">
-        <v>42272</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A14" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="D14" s="26" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A15" s="19">
-        <v>42275</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="26"/>
-    </row>
-    <row r="16" spans="1:5" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A16" s="19">
-        <v>42275</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="D16" s="26" t="s">
+    <row r="29" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A29" s="54">
+        <v>42310</v>
+      </c>
+      <c r="B29" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="45"/>
+    </row>
+    <row r="30" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A30" s="54">
+        <v>42317</v>
+      </c>
+      <c r="B30" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="45"/>
+    </row>
+    <row r="31" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A31" s="54">
+        <v>42324</v>
+      </c>
+      <c r="B31" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="45"/>
+    </row>
+    <row r="32" spans="1:5" s="19" customFormat="1" ht="30" customHeight="1">
+      <c r="A32" s="54">
+        <v>42331</v>
+      </c>
+      <c r="B32" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="45"/>
+    </row>
+    <row r="33" spans="1:4" s="19" customFormat="1" ht="30" customHeight="1">
+      <c r="A33" s="54">
+        <v>42338</v>
+      </c>
+      <c r="B33" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="45"/>
+    </row>
+    <row r="34" spans="1:4" s="19" customFormat="1" ht="30" customHeight="1">
+      <c r="A34" s="54">
+        <v>42345</v>
+      </c>
+      <c r="B34" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="45"/>
+    </row>
+    <row r="35" spans="1:4" s="19" customFormat="1" ht="30" customHeight="1">
+      <c r="A35" s="54">
+        <v>42345</v>
+      </c>
+      <c r="B35" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="45" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A17" s="19">
-        <v>42279</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="D17" s="26" t="s">
+    <row r="36" spans="1:4" s="19" customFormat="1" ht="30" customHeight="1">
+      <c r="A36" s="54">
+        <v>42352</v>
+      </c>
+      <c r="B36" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="D36" s="45" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A18" s="19">
-        <v>42282</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="26"/>
-    </row>
-    <row r="19" spans="1:4" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A19" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="26"/>
-    </row>
-    <row r="20" spans="1:4" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A20" s="19">
-        <v>42286</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A21" s="19">
-        <v>42289</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="26"/>
-    </row>
-    <row r="22" spans="1:4" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A22" s="19"/>
-      <c r="B22" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="26"/>
-    </row>
-    <row r="23" spans="1:4" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A23" s="19"/>
-      <c r="B23" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="26"/>
-    </row>
-    <row r="24" spans="1:4" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A24" s="19">
-        <v>42296</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="26"/>
-    </row>
-    <row r="25" spans="1:4" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A25" s="19"/>
-      <c r="B25" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="26"/>
-    </row>
-    <row r="26" spans="1:4" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A26" s="19"/>
-      <c r="B26" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="26"/>
-    </row>
-    <row r="27" spans="1:4" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A27" s="19">
-        <v>42303</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="26"/>
-    </row>
-    <row r="28" spans="1:4" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A28" s="19"/>
-      <c r="B28" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="26"/>
-    </row>
-    <row r="29" spans="1:4" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A29" s="19"/>
-      <c r="B29" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" s="26"/>
-    </row>
-    <row r="30" spans="1:4" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A30" s="19">
-        <v>42310</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30" s="26"/>
-    </row>
-    <row r="31" spans="1:4" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A31" s="19">
-        <v>42317</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="26"/>
-    </row>
-    <row r="32" spans="1:4" s="24" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A32" s="19">
-        <v>42324</v>
-      </c>
-      <c r="B32" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32" s="26"/>
-    </row>
-    <row r="33" spans="1:4" s="24" customFormat="1" ht="30" customHeight="1">
-      <c r="A33" s="19">
-        <v>42331</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="D33" s="26"/>
-    </row>
-    <row r="34" spans="1:4" s="24" customFormat="1" ht="30" customHeight="1">
-      <c r="A34" s="19">
-        <v>42338</v>
-      </c>
-      <c r="B34" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34" s="26"/>
-    </row>
-    <row r="35" spans="1:4" s="24" customFormat="1" ht="30" customHeight="1">
-      <c r="A35" s="19">
-        <v>42345</v>
-      </c>
-      <c r="B35" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="D35" s="26"/>
-    </row>
-    <row r="36" spans="1:4" s="24" customFormat="1" ht="30" customHeight="1">
-      <c r="A36" s="29">
-        <v>42345</v>
-      </c>
-      <c r="B36" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C36" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D36" s="26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" s="24" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A37" s="21">
-        <v>42352</v>
-      </c>
-      <c r="B37" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C37" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="D37" s="26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" s="25" customFormat="1" thickTop="1">
-      <c r="D38" s="27"/>
-    </row>
-    <row r="39" spans="1:4" s="25" customFormat="1" ht="12">
-      <c r="D39" s="27"/>
-    </row>
-    <row r="40" spans="1:4" s="25" customFormat="1" ht="12">
-      <c r="D40" s="27"/>
-    </row>
-    <row r="41" spans="1:4" s="25" customFormat="1" ht="12">
-      <c r="D41" s="27"/>
-    </row>
-    <row r="42" spans="1:4" s="25" customFormat="1" ht="12">
-      <c r="D42" s="27"/>
-    </row>
-    <row r="43" spans="1:4" s="25" customFormat="1" ht="12">
-      <c r="D43" s="27"/>
-    </row>
-    <row r="44" spans="1:4" s="25" customFormat="1" ht="12">
-      <c r="D44" s="27"/>
-    </row>
-    <row r="45" spans="1:4" s="25" customFormat="1" ht="12">
-      <c r="D45" s="27"/>
-    </row>
-    <row r="46" spans="1:4" s="25" customFormat="1" ht="12">
-      <c r="D46" s="27"/>
-    </row>
-    <row r="47" spans="1:4" s="25" customFormat="1" ht="12">
-      <c r="D47" s="27"/>
-    </row>
-    <row r="48" spans="1:4" s="25" customFormat="1" ht="12">
-      <c r="D48" s="27"/>
-    </row>
-    <row r="49" spans="4:4" s="25" customFormat="1" ht="12">
-      <c r="D49" s="27"/>
-    </row>
-    <row r="50" spans="4:4" s="25" customFormat="1" ht="12">
-      <c r="D50" s="27"/>
-    </row>
-    <row r="51" spans="4:4" s="25" customFormat="1" ht="12">
-      <c r="D51" s="27"/>
-    </row>
-    <row r="52" spans="4:4" s="25" customFormat="1" ht="12">
-      <c r="D52" s="27"/>
-    </row>
-    <row r="53" spans="4:4" s="25" customFormat="1" ht="12">
-      <c r="D53" s="27"/>
-    </row>
-    <row r="54" spans="4:4" s="25" customFormat="1" ht="12">
-      <c r="D54" s="27"/>
-    </row>
-    <row r="55" spans="4:4" s="25" customFormat="1" ht="12">
-      <c r="D55" s="27"/>
+    <row r="37" spans="1:4" s="20" customFormat="1" ht="12">
+      <c r="A37" s="58"/>
+      <c r="B37" s="59"/>
+      <c r="D37" s="47"/>
+    </row>
+    <row r="38" spans="1:4" s="20" customFormat="1" ht="12">
+      <c r="A38" s="58"/>
+      <c r="B38" s="59"/>
+      <c r="D38" s="47"/>
+    </row>
+    <row r="39" spans="1:4" s="20" customFormat="1" ht="12">
+      <c r="A39" s="58"/>
+      <c r="B39" s="59"/>
+      <c r="D39" s="47"/>
+    </row>
+    <row r="40" spans="1:4" s="20" customFormat="1" ht="12">
+      <c r="A40" s="58"/>
+      <c r="B40" s="59"/>
+      <c r="D40" s="47"/>
+    </row>
+    <row r="41" spans="1:4" s="20" customFormat="1" ht="12">
+      <c r="A41" s="58"/>
+      <c r="B41" s="59"/>
+      <c r="D41" s="47"/>
+    </row>
+    <row r="42" spans="1:4" s="20" customFormat="1" ht="12">
+      <c r="A42" s="58"/>
+      <c r="B42" s="59"/>
+      <c r="D42" s="47"/>
+    </row>
+    <row r="43" spans="1:4" s="20" customFormat="1" ht="12">
+      <c r="A43" s="58"/>
+      <c r="B43" s="59"/>
+      <c r="D43" s="47"/>
+    </row>
+    <row r="44" spans="1:4" s="20" customFormat="1" ht="12">
+      <c r="A44" s="58"/>
+      <c r="B44" s="59"/>
+      <c r="D44" s="47"/>
+    </row>
+    <row r="45" spans="1:4" s="20" customFormat="1" ht="12">
+      <c r="A45" s="58"/>
+      <c r="B45" s="59"/>
+      <c r="D45" s="47"/>
+    </row>
+    <row r="46" spans="1:4" s="20" customFormat="1" ht="12">
+      <c r="A46" s="58"/>
+      <c r="B46" s="59"/>
+      <c r="D46" s="47"/>
+    </row>
+    <row r="47" spans="1:4" s="20" customFormat="1" ht="12">
+      <c r="A47" s="58"/>
+      <c r="B47" s="59"/>
+      <c r="D47" s="47"/>
+    </row>
+    <row r="48" spans="1:4" s="20" customFormat="1" ht="12">
+      <c r="A48" s="58"/>
+      <c r="B48" s="59"/>
+      <c r="D48" s="47"/>
+    </row>
+    <row r="49" spans="1:4" s="20" customFormat="1" ht="12">
+      <c r="A49" s="58"/>
+      <c r="B49" s="59"/>
+      <c r="D49" s="47"/>
+    </row>
+    <row r="50" spans="1:4" s="20" customFormat="1" ht="12">
+      <c r="A50" s="58"/>
+      <c r="B50" s="59"/>
+      <c r="D50" s="47"/>
+    </row>
+    <row r="51" spans="1:4" s="20" customFormat="1" ht="12">
+      <c r="A51" s="58"/>
+      <c r="B51" s="59"/>
+      <c r="D51" s="47"/>
+    </row>
+    <row r="52" spans="1:4" s="20" customFormat="1" ht="12">
+      <c r="A52" s="58"/>
+      <c r="B52" s="59"/>
+      <c r="D52" s="47"/>
+    </row>
+    <row r="53" spans="1:4" s="20" customFormat="1" ht="12">
+      <c r="A53" s="58"/>
+      <c r="B53" s="59"/>
+      <c r="D53" s="47"/>
+    </row>
+    <row r="54" spans="1:4" s="20" customFormat="1" ht="12">
+      <c r="A54" s="58"/>
+      <c r="B54" s="59"/>
+      <c r="D54" s="47"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>
@@ -3436,7 +3581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D35"/>
     </sheetView>
   </sheetViews>
@@ -3449,366 +3594,366 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="13">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="32" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="13">
+      <c r="A2" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="B2" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="13">
-      <c r="A2" s="34" t="s">
+    <row r="3" spans="1:4" ht="13">
+      <c r="A3" s="23"/>
+      <c r="B3" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+    </row>
+    <row r="4" spans="1:4" ht="13">
+      <c r="A4" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35" t="s">
+      <c r="B4" s="26" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="13">
-      <c r="A3" s="34"/>
-      <c r="B3" s="35" t="s">
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+    </row>
+    <row r="5" spans="1:4" ht="13">
+      <c r="A5" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-    </row>
-    <row r="4" spans="1:4" ht="13">
-      <c r="A4" s="36" t="s">
+      <c r="B5" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="C5" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-    </row>
-    <row r="5" spans="1:4" ht="13">
-      <c r="A5" s="34" t="s">
+      <c r="D5" s="24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="13">
+      <c r="A6" s="23"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+    </row>
+    <row r="7" spans="1:4" ht="13">
+      <c r="A7" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B7" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C7" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="35" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="13">
-      <c r="A6" s="34"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-    </row>
-    <row r="7" spans="1:4" ht="13">
-      <c r="A7" s="39" t="s">
+      <c r="D7" s="29"/>
+    </row>
+    <row r="8" spans="1:4" ht="13">
+      <c r="A8" s="23"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="D8" s="24"/>
+    </row>
+    <row r="9" spans="1:4" ht="13">
+      <c r="A9" s="30"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="D9" s="31"/>
+    </row>
+    <row r="10" spans="1:4" ht="15">
+      <c r="A10" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="40"/>
-    </row>
-    <row r="8" spans="1:4" ht="13">
-      <c r="A8" s="34"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35" t="s">
+      <c r="B10" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="35"/>
-    </row>
-    <row r="9" spans="1:4" ht="13">
-      <c r="A9" s="41"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="43" t="s">
+      <c r="C10" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="13">
+      <c r="A11" s="23"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="24"/>
+    </row>
+    <row r="12" spans="1:4" ht="13">
+      <c r="A12" s="23"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="42"/>
-    </row>
-    <row r="10" spans="1:4" ht="15">
-      <c r="A10" s="34" t="s">
+      <c r="D12" s="24"/>
+    </row>
+    <row r="13" spans="1:4" ht="13">
+      <c r="A13" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B13" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="13">
+      <c r="A14" s="30"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="31"/>
+    </row>
+    <row r="15" spans="1:4" ht="13">
+      <c r="A15" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="35" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="13">
-      <c r="A11" s="34"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="35"/>
-    </row>
-    <row r="12" spans="1:4" ht="13">
-      <c r="A12" s="34"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="38" t="s">
+      <c r="B15" s="24"/>
+      <c r="C15" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="35"/>
-    </row>
-    <row r="13" spans="1:4" ht="13">
-      <c r="A13" s="39" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="13">
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="40" t="s">
+    </row>
+    <row r="17" spans="1:4" ht="13">
+      <c r="A17" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="13">
+      <c r="A18" s="30"/>
+      <c r="B18" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="31"/>
+    </row>
+    <row r="19" spans="1:4" ht="13">
+      <c r="A19" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="24"/>
+    </row>
+    <row r="20" spans="1:4" ht="13">
+      <c r="A20" s="23"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="24"/>
+    </row>
+    <row r="21" spans="1:4" ht="13">
+      <c r="A21" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="13">
+      <c r="A22" s="30"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="13">
+      <c r="A23" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="24"/>
+    </row>
+    <row r="24" spans="1:4" ht="13">
+      <c r="A24" s="23"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+    </row>
+    <row r="25" spans="1:4" ht="13">
+      <c r="A25" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="13">
+      <c r="A26" s="37"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="31"/>
+    </row>
+    <row r="27" spans="1:4" ht="13">
+      <c r="A27" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="24"/>
+    </row>
+    <row r="28" spans="1:4" ht="13">
+      <c r="A28" s="30"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="24"/>
+    </row>
+    <row r="29" spans="1:4" ht="13">
+      <c r="A29" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="29"/>
+    </row>
+    <row r="30" spans="1:4" ht="13">
+      <c r="A30" s="30"/>
+      <c r="B30" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="31"/>
+    </row>
+    <row r="31" spans="1:4" ht="13">
+      <c r="A31" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="40" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="13">
-      <c r="A14" s="41"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="42"/>
-    </row>
-    <row r="15" spans="1:4" ht="13">
-      <c r="A15" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="35" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="13">
-      <c r="A16" s="34"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="35" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="13">
-      <c r="A17" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="40" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="13">
-      <c r="A18" s="41"/>
-      <c r="B18" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="C18" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="42"/>
-    </row>
-    <row r="19" spans="1:4" ht="13">
-      <c r="A19" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="35"/>
-    </row>
-    <row r="20" spans="1:4" ht="13">
-      <c r="A20" s="34"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="35"/>
-    </row>
-    <row r="21" spans="1:4" ht="13">
-      <c r="A21" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" s="40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="13">
-      <c r="A22" s="41"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="43" t="s">
-        <v>77</v>
-      </c>
-      <c r="D22" s="42" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="13">
-      <c r="A23" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="C23" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" s="35"/>
-    </row>
-    <row r="24" spans="1:4" ht="13">
-      <c r="A24" s="34"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-    </row>
-    <row r="25" spans="1:4" ht="13">
-      <c r="A25" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="C25" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="40" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="13">
-      <c r="A26" s="48"/>
-      <c r="B26" s="49"/>
-      <c r="C26" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="42"/>
-    </row>
-    <row r="27" spans="1:4" ht="13">
-      <c r="A27" s="46" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" s="47" t="s">
+      <c r="C31" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="24"/>
+    </row>
+    <row r="32" spans="1:4" ht="13">
+      <c r="A32" s="23"/>
+      <c r="B32" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" s="35"/>
-    </row>
-    <row r="28" spans="1:4" ht="13">
-      <c r="A28" s="41"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="D28" s="35"/>
-    </row>
-    <row r="29" spans="1:4" ht="13">
-      <c r="A29" s="39" t="s">
+      <c r="D32" s="24"/>
+    </row>
+    <row r="33" spans="1:4" ht="13">
+      <c r="A33" s="30"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="B29" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" s="40"/>
-    </row>
-    <row r="30" spans="1:4" ht="13">
-      <c r="A30" s="41"/>
-      <c r="B30" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="C30" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="42"/>
-    </row>
-    <row r="31" spans="1:4" ht="13">
-      <c r="A31" s="34" t="s">
+      <c r="D33" s="24"/>
+    </row>
+    <row r="34" spans="1:4" ht="13">
+      <c r="A34" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="B31" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="C31" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="35"/>
-    </row>
-    <row r="32" spans="1:4" ht="13">
-      <c r="A32" s="34"/>
-      <c r="B32" s="35" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" s="35" t="s">
+      <c r="B34" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="D32" s="35"/>
-    </row>
-    <row r="33" spans="1:4" ht="13">
-      <c r="A33" s="41"/>
-      <c r="B33" s="42"/>
-      <c r="C33" s="42" t="s">
+      <c r="C34" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="D33" s="35"/>
-    </row>
-    <row r="34" spans="1:4" ht="13">
-      <c r="A34" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="B34" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="D34" s="40"/>
+      <c r="D34" s="29"/>
     </row>
     <row r="35" spans="1:4" ht="13">
-      <c r="A35" s="41"/>
-      <c r="B35" s="42"/>
-      <c r="C35" s="42" t="s">
-        <v>88</v>
-      </c>
-      <c r="D35" s="42"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3834,83 +3979,83 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="50"/>
-    <col min="2" max="2" width="22.33203125" style="50" customWidth="1"/>
-    <col min="3" max="3" width="46" style="50" customWidth="1"/>
-    <col min="4" max="4" width="72.83203125" style="50" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="50"/>
+    <col min="1" max="1" width="8.83203125" style="39"/>
+    <col min="2" max="2" width="22.33203125" style="39" customWidth="1"/>
+    <col min="3" max="3" width="46" style="39" customWidth="1"/>
+    <col min="4" max="4" width="72.83203125" style="39" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="39" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="39" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="53" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="51" t="s">
+      <c r="D3" s="39" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="41" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A4" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+    </row>
+    <row r="5" spans="1:4" s="41" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A5" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+    </row>
+    <row r="6" spans="1:4" s="41" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A6" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="50" t="s">
-        <v>100</v>
-      </c>
-      <c r="D3" s="50" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="52" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A4" s="54" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-    </row>
-    <row r="5" spans="1:4" s="52" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A5" s="54" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-    </row>
-    <row r="6" spans="1:4" s="52" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A6" s="54" t="s">
-        <v>102</v>
-      </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-    </row>
-    <row r="7" spans="1:4" s="52" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A7" s="54"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-    </row>
-    <row r="8" spans="1:4" s="52" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A8" s="54"/>
-      <c r="B8" s="55"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-    </row>
-    <row r="9" spans="1:4" s="52" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A9" s="54"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-    </row>
-    <row r="10" spans="1:4" s="52" customFormat="1"/>
-    <row r="11" spans="1:4" s="52" customFormat="1"/>
-    <row r="12" spans="1:4" s="52" customFormat="1"/>
-    <row r="13" spans="1:4" s="52" customFormat="1"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+    </row>
+    <row r="7" spans="1:4" s="41" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A7" s="43"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+    </row>
+    <row r="8" spans="1:4" s="41" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A8" s="43"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+    </row>
+    <row r="9" spans="1:4" s="41" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A9" s="43"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+    </row>
+    <row r="10" spans="1:4" s="41" customFormat="1"/>
+    <row r="11" spans="1:4" s="41" customFormat="1"/>
+    <row r="12" spans="1:4" s="41" customFormat="1"/>
+    <row r="13" spans="1:4" s="41" customFormat="1"/>
   </sheetData>
   <conditionalFormatting sqref="A4:A8">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">

</xml_diff>

<commit_message>
Start UML doc + week update
started UML documentation and filled out weekly report
</commit_message>
<xml_diff>
--- a/HW 1/Project Plan Template.xlsx
+++ b/HW 1/Project Plan Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="0" windowWidth="25260" windowHeight="12200" activeTab="2"/>
+    <workbookView xWindow="180" yWindow="0" windowWidth="25260" windowHeight="12200" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Project Timeline" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="153">
   <si>
     <t>Project Start</t>
   </si>
@@ -493,6 +493,24 @@
   </si>
   <si>
     <t>Put em in a coffin entire thing is AWPerational</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project plan </t>
+  </si>
+  <si>
+    <t>Our layout and milestones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We had a long discussion about if the milestones are duedates or if they are more of a meeting schedule. </t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Looking for what the layout should look like</t>
+  </si>
+  <si>
+    <t>Should the documentation be in one massive pdf or separate word docs? Also is there a certain way they should be laid out?</t>
   </si>
 </sst>
 </file>
@@ -928,7 +946,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1097,6 +1115,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="5" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="21">
@@ -1757,8 +1778,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2120554024"/>
-        <c:axId val="2120551080"/>
+        <c:axId val="2085835224"/>
+        <c:axId val="2085832280"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1929,11 +1950,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2120544376"/>
-        <c:axId val="2120548008"/>
+        <c:axId val="2085841736"/>
+        <c:axId val="2085829160"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2120544376"/>
+        <c:axId val="2085841736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1973,7 +1994,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2120548008"/>
+        <c:crossAx val="2085829160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1984,7 +2005,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2120548008"/>
+        <c:axId val="2085829160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1994,12 +2015,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2120544376"/>
+        <c:crossAx val="2085841736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2120551080"/>
+        <c:axId val="2085832280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2009,12 +2030,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2120554024"/>
+        <c:crossAx val="2085835224"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2120554024"/>
+        <c:axId val="2085835224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2024,7 +2045,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2120551080"/>
+        <c:crossAx val="2085832280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2967,7 +2988,7 @@
   </sheetPr>
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -3581,7 +3602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D35"/>
     </sheetView>
   </sheetViews>
@@ -3974,7 +3995,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -3995,6 +4016,9 @@
       <c r="A2" s="42" t="s">
         <v>24</v>
       </c>
+      <c r="B2" s="63">
+        <v>42252</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="40" t="s">
@@ -4014,17 +4038,29 @@
       <c r="A4" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
+      <c r="B4" s="44" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="5" spans="1:4" s="41" customFormat="1" ht="38.25" customHeight="1">
       <c r="A5" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
+      <c r="B5" s="44" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="6" spans="1:4" s="41" customFormat="1" ht="38.25" customHeight="1">
       <c r="A6" s="43" t="s">

</xml_diff>